<commit_message>
caught the error in the value in put 0.73 but its 7.30
</commit_message>
<xml_diff>
--- a/Cosmetics Inc. - Data for Pivot Table and VLOOKUP.xlsx
+++ b/Cosmetics Inc. - Data for Pivot Table and VLOOKUP.xlsx
@@ -568,11 +568,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="771934177"/>
-        <c:axId val="2138225468"/>
+        <c:axId val="1013890479"/>
+        <c:axId val="1422703251"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="771934177"/>
+        <c:axId val="1013890479"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -624,10 +624,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2138225468"/>
+        <c:crossAx val="1422703251"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2138225468"/>
+        <c:axId val="1422703251"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -702,7 +702,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="771934177"/>
+        <c:crossAx val="1013890479"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -732,10 +732,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
@@ -791,7 +791,7 @@
         <n v="7.58"/>
         <n v="11.75"/>
         <n v="10.95"/>
-        <n v="0.73"/>
+        <n v="7.3"/>
         <n v="6.66"/>
         <n v="12.06"/>
         <n v="12.95"/>
@@ -1583,7 +1583,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="4">
-        <v>0.73</v>
+        <v>7.3</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>8</v>

</xml_diff>